<commit_message>
Base de datos con filas ENORMES por sujeto
</commit_message>
<xml_diff>
--- a/Proyectos/Mario_BisecciónTemporal/Datos_Sujeto3.xlsx
+++ b/Proyectos/Mario_BisecciónTemporal/Datos_Sujeto3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\Felisa\Proyectos\Mario_BisecciónTemporal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana\Desktop\Felisa\Proyectos\Mario_BisecciónTemporal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,36 +98,24 @@
     <t>LBSignal_7</t>
   </si>
   <si>
-    <t>LBNoise_7</t>
-  </si>
-  <si>
     <t>LBF_8</t>
   </si>
   <si>
     <t>LBSignal_8</t>
   </si>
   <si>
-    <t>LBNoise_8</t>
-  </si>
-  <si>
     <t>LBF_9</t>
   </si>
   <si>
     <t>LBSignal_9</t>
   </si>
   <si>
-    <t>LBNoise_9</t>
-  </si>
-  <si>
     <t>LBF_10</t>
   </si>
   <si>
     <t>LBSignal_10</t>
   </si>
   <si>
-    <t>LBNoise_10</t>
-  </si>
-  <si>
     <t>Condicion</t>
   </si>
   <si>
@@ -140,9 +128,6 @@
     <t>MSignal_1</t>
   </si>
   <si>
-    <t>MNoise_1</t>
-  </si>
-  <si>
     <t>MH_2</t>
   </si>
   <si>
@@ -152,9 +137,6 @@
     <t>MSignal_2</t>
   </si>
   <si>
-    <t>MNoise_2</t>
-  </si>
-  <si>
     <t>MH_3</t>
   </si>
   <si>
@@ -164,9 +146,6 @@
     <t>MSignal_3</t>
   </si>
   <si>
-    <t>MNoise_3</t>
-  </si>
-  <si>
     <t>MH_4</t>
   </si>
   <si>
@@ -176,9 +155,6 @@
     <t>MSignal_4</t>
   </si>
   <si>
-    <t>MNoise_4</t>
-  </si>
-  <si>
     <t>MH_5</t>
   </si>
   <si>
@@ -188,9 +164,6 @@
     <t>MSignal_5</t>
   </si>
   <si>
-    <t>MNoise_5</t>
-  </si>
-  <si>
     <t>MH_6</t>
   </si>
   <si>
@@ -200,9 +173,6 @@
     <t>MSignal_6</t>
   </si>
   <si>
-    <t>MNoise_6</t>
-  </si>
-  <si>
     <t>MH_7</t>
   </si>
   <si>
@@ -212,9 +182,6 @@
     <t>MSignal_7</t>
   </si>
   <si>
-    <t>MNoise_7</t>
-  </si>
-  <si>
     <t>MH_8</t>
   </si>
   <si>
@@ -224,9 +191,6 @@
     <t>MSignal_8</t>
   </si>
   <si>
-    <t>MNoise_8</t>
-  </si>
-  <si>
     <t>MH_9</t>
   </si>
   <si>
@@ -236,9 +200,6 @@
     <t>MSignal_9</t>
   </si>
   <si>
-    <t>MNoise_9</t>
-  </si>
-  <si>
     <t>MH_10</t>
   </si>
   <si>
@@ -248,9 +209,6 @@
     <t>MSignal_10</t>
   </si>
   <si>
-    <t>MNoise_10</t>
-  </si>
-  <si>
     <t>1v4</t>
   </si>
   <si>
@@ -279,6 +237,48 @@
   </si>
   <si>
     <t>LBR_6</t>
+  </si>
+  <si>
+    <t>MR_10</t>
+  </si>
+  <si>
+    <t>MR_9</t>
+  </si>
+  <si>
+    <t>MR_8</t>
+  </si>
+  <si>
+    <t>MR_7</t>
+  </si>
+  <si>
+    <t>MR_6</t>
+  </si>
+  <si>
+    <t>MR_5</t>
+  </si>
+  <si>
+    <t>MR_4</t>
+  </si>
+  <si>
+    <t>MR_3</t>
+  </si>
+  <si>
+    <t>MR_2</t>
+  </si>
+  <si>
+    <t>MR_1</t>
+  </si>
+  <si>
+    <t>LBR_10</t>
+  </si>
+  <si>
+    <t>LBR_9</t>
+  </si>
+  <si>
+    <t>LBR_8</t>
+  </si>
+  <si>
+    <t>LBR_7</t>
   </si>
 </sst>
 </file>
@@ -598,21 +598,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" workbookViewId="0">
+      <selection activeCell="CD5" sqref="CD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
@@ -636,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
@@ -648,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="P1" t="s">
         <v>16</v>
@@ -660,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="S1" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="T1" t="s">
         <v>18</v>
@@ -672,7 +672,7 @@
         <v>5</v>
       </c>
       <c r="W1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="X1" t="s">
         <v>20</v>
@@ -684,174 +684,174 @@
         <v>6</v>
       </c>
       <c r="AA1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
       </c>
       <c r="AD1" t="s">
         <v>7</v>
       </c>
       <c r="AE1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG1" t="s">
         <v>25</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>27</v>
       </c>
       <c r="AH1" t="s">
         <v>8</v>
       </c>
       <c r="AI1" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="AJ1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AK1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AL1" t="s">
         <v>9</v>
       </c>
       <c r="AM1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR1" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AS1" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AT1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV1" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AW1" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AX1" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AY1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BA1" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BB1" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BC1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD1" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BE1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BF1" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BG1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH1" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BI1" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BJ1" t="s">
         <v>46</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BK1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL1" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BM1" t="s">
         <v>48</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BN1" t="s">
         <v>49</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BO1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BP1" t="s">
         <v>50</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BQ1" t="s">
         <v>51</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BR1" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BS1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BT1" t="s">
         <v>53</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BU1" t="s">
         <v>54</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BV1" t="s">
         <v>55</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BW1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BX1" t="s">
         <v>56</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BY1" t="s">
         <v>57</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BZ1" t="s">
         <v>58</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="CA1" t="s">
+        <v>71</v>
+      </c>
+      <c r="CB1" t="s">
         <v>59</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="CC1" t="s">
         <v>60</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>72</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>73</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>54</v>
@@ -859,6 +859,9 @@
       <c r="C2">
         <v>48</v>
       </c>
+      <c r="D2">
+        <v>28</v>
+      </c>
       <c r="E2">
         <v>55</v>
       </c>
@@ -868,6 +871,9 @@
       <c r="G2">
         <v>55</v>
       </c>
+      <c r="H2">
+        <v>35</v>
+      </c>
       <c r="I2">
         <v>51</v>
       </c>
@@ -877,6 +883,9 @@
       <c r="K2">
         <v>47</v>
       </c>
+      <c r="L2">
+        <v>33</v>
+      </c>
       <c r="M2">
         <v>52</v>
       </c>
@@ -886,6 +895,9 @@
       <c r="O2">
         <v>45</v>
       </c>
+      <c r="P2">
+        <v>29</v>
+      </c>
       <c r="Q2">
         <v>47</v>
       </c>
@@ -895,15 +907,21 @@
       <c r="S2">
         <v>33</v>
       </c>
+      <c r="T2">
+        <v>13</v>
+      </c>
       <c r="U2">
         <v>40</v>
       </c>
       <c r="V2">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="W2">
         <v>35</v>
       </c>
+      <c r="X2">
+        <v>27</v>
+      </c>
       <c r="Y2">
         <v>36</v>
       </c>
@@ -914,10 +932,10 @@
         <v>44</v>
       </c>
       <c r="AB2">
+        <v>34</v>
+      </c>
+      <c r="AC2">
         <v>47</v>
-      </c>
-      <c r="AC2">
-        <v>44</v>
       </c>
       <c r="AD2">
         <v>50</v>
@@ -926,10 +944,10 @@
         <v>38</v>
       </c>
       <c r="AF2">
+        <v>32</v>
+      </c>
+      <c r="AG2">
         <v>52</v>
-      </c>
-      <c r="AG2">
-        <v>41</v>
       </c>
       <c r="AH2">
         <v>47</v>
@@ -938,10 +956,10 @@
         <v>54</v>
       </c>
       <c r="AJ2">
+        <v>48</v>
+      </c>
+      <c r="AK2">
         <v>49</v>
-      </c>
-      <c r="AK2">
-        <v>56</v>
       </c>
       <c r="AL2">
         <v>55</v>
@@ -950,10 +968,10 @@
         <v>56</v>
       </c>
       <c r="AN2">
+        <v>48</v>
+      </c>
+      <c r="AO2">
         <v>59</v>
-      </c>
-      <c r="AO2">
-        <v>58</v>
       </c>
       <c r="AP2">
         <v>43</v>
@@ -962,10 +980,10 @@
         <v>48</v>
       </c>
       <c r="AR2">
+        <v>30</v>
+      </c>
+      <c r="AS2">
         <v>43</v>
-      </c>
-      <c r="AS2">
-        <v>49</v>
       </c>
       <c r="AT2">
         <v>39</v>
@@ -974,10 +992,10 @@
         <v>36</v>
       </c>
       <c r="AV2">
+        <v>18</v>
+      </c>
+      <c r="AW2">
         <v>43</v>
-      </c>
-      <c r="AW2">
-        <v>40</v>
       </c>
       <c r="AX2">
         <v>33</v>
@@ -986,10 +1004,10 @@
         <v>39</v>
       </c>
       <c r="AZ2">
+        <v>19</v>
+      </c>
+      <c r="BA2">
         <v>36</v>
-      </c>
-      <c r="BA2">
-        <v>39</v>
       </c>
       <c r="BB2">
         <v>49</v>
@@ -998,10 +1016,10 @@
         <v>47</v>
       </c>
       <c r="BD2">
+        <v>29</v>
+      </c>
+      <c r="BE2">
         <v>52</v>
-      </c>
-      <c r="BE2">
-        <v>49</v>
       </c>
       <c r="BF2">
         <v>44</v>
@@ -1010,10 +1028,10 @@
         <v>47</v>
       </c>
       <c r="BH2">
+        <v>31</v>
+      </c>
+      <c r="BI2">
         <v>45</v>
-      </c>
-      <c r="BI2">
-        <v>49</v>
       </c>
       <c r="BJ2">
         <v>43</v>
@@ -1022,10 +1040,10 @@
         <v>48</v>
       </c>
       <c r="BL2">
+        <v>30</v>
+      </c>
+      <c r="BM2">
         <v>47</v>
-      </c>
-      <c r="BM2">
-        <v>50</v>
       </c>
       <c r="BN2">
         <v>48</v>
@@ -1034,10 +1052,10 @@
         <v>27</v>
       </c>
       <c r="BP2">
+        <v>25</v>
+      </c>
+      <c r="BQ2">
         <v>51</v>
-      </c>
-      <c r="BQ2">
-        <v>47</v>
       </c>
       <c r="BR2">
         <v>51</v>
@@ -1046,10 +1064,10 @@
         <v>49</v>
       </c>
       <c r="BT2">
+        <v>31</v>
+      </c>
+      <c r="BU2">
         <v>52</v>
-      </c>
-      <c r="BU2">
-        <v>51</v>
       </c>
       <c r="BV2">
         <v>43</v>
@@ -1058,10 +1076,10 @@
         <v>38</v>
       </c>
       <c r="BX2">
+        <v>20</v>
+      </c>
+      <c r="BY2">
         <v>44</v>
-      </c>
-      <c r="BY2">
-        <v>40</v>
       </c>
       <c r="BZ2">
         <v>35</v>
@@ -1070,15 +1088,15 @@
         <v>38</v>
       </c>
       <c r="CB2">
+        <v>18</v>
+      </c>
+      <c r="CC2">
         <v>40</v>
-      </c>
-      <c r="CC2">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>43</v>
@@ -1086,6 +1104,9 @@
       <c r="C3">
         <v>34</v>
       </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
       <c r="E3">
         <v>45</v>
       </c>
@@ -1095,6 +1116,9 @@
       <c r="G3">
         <v>36</v>
       </c>
+      <c r="H3">
+        <v>22</v>
+      </c>
       <c r="I3">
         <v>33</v>
       </c>
@@ -1104,6 +1128,9 @@
       <c r="K3">
         <v>32</v>
       </c>
+      <c r="L3">
+        <v>16</v>
+      </c>
       <c r="M3">
         <v>29</v>
       </c>
@@ -1113,6 +1140,9 @@
       <c r="O3">
         <v>31</v>
       </c>
+      <c r="P3">
+        <v>17</v>
+      </c>
       <c r="Q3">
         <v>34</v>
       </c>
@@ -1122,6 +1152,9 @@
       <c r="S3">
         <v>41</v>
       </c>
+      <c r="T3">
+        <v>35</v>
+      </c>
       <c r="U3">
         <v>46</v>
       </c>
@@ -1131,6 +1164,9 @@
       <c r="W3">
         <v>39</v>
       </c>
+      <c r="X3">
+        <v>31</v>
+      </c>
       <c r="Y3">
         <v>36</v>
       </c>
@@ -1141,10 +1177,10 @@
         <v>32</v>
       </c>
       <c r="AB3">
+        <v>24</v>
+      </c>
+      <c r="AC3">
         <v>35</v>
-      </c>
-      <c r="AC3">
-        <v>32</v>
       </c>
       <c r="AD3">
         <v>33</v>
@@ -1153,10 +1189,10 @@
         <v>26</v>
       </c>
       <c r="AF3">
+        <v>18</v>
+      </c>
+      <c r="AG3">
         <v>36</v>
-      </c>
-      <c r="AG3">
-        <v>33</v>
       </c>
       <c r="AH3">
         <v>34</v>
@@ -1165,10 +1201,10 @@
         <v>38</v>
       </c>
       <c r="AJ3">
+        <v>36</v>
+      </c>
+      <c r="AK3">
         <v>37</v>
-      </c>
-      <c r="AK3">
-        <v>41</v>
       </c>
       <c r="AL3">
         <v>31</v>
@@ -1177,10 +1213,10 @@
         <v>25</v>
       </c>
       <c r="AN3">
+        <v>19</v>
+      </c>
+      <c r="AO3">
         <v>33</v>
-      </c>
-      <c r="AO3">
-        <v>28</v>
       </c>
       <c r="AP3">
         <v>29</v>
@@ -1189,7 +1225,7 @@
         <v>32</v>
       </c>
       <c r="AR3">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="AS3">
         <v>32</v>
@@ -1201,10 +1237,10 @@
         <v>40</v>
       </c>
       <c r="AV3">
+        <v>25</v>
+      </c>
+      <c r="AW3">
         <v>46</v>
-      </c>
-      <c r="AW3">
-        <v>41</v>
       </c>
       <c r="AX3">
         <v>31</v>
@@ -1213,10 +1249,10 @@
         <v>32</v>
       </c>
       <c r="AZ3">
+        <v>22</v>
+      </c>
+      <c r="BA3">
         <v>36</v>
-      </c>
-      <c r="BA3">
-        <v>35</v>
       </c>
       <c r="BB3">
         <v>31</v>
@@ -1225,10 +1261,10 @@
         <v>33</v>
       </c>
       <c r="BD3">
+        <v>23</v>
+      </c>
+      <c r="BE3">
         <v>35</v>
-      </c>
-      <c r="BE3">
-        <v>37</v>
       </c>
       <c r="BF3">
         <v>26</v>
@@ -1237,10 +1273,10 @@
         <v>15</v>
       </c>
       <c r="BH3">
+        <v>15</v>
+      </c>
+      <c r="BI3">
         <v>28</v>
-      </c>
-      <c r="BI3">
-        <v>31</v>
       </c>
       <c r="BJ3">
         <v>33</v>
@@ -1249,10 +1285,10 @@
         <v>32</v>
       </c>
       <c r="BL3">
+        <v>24</v>
+      </c>
+      <c r="BM3">
         <v>37</v>
-      </c>
-      <c r="BM3">
-        <v>35</v>
       </c>
       <c r="BN3">
         <v>32</v>
@@ -1261,10 +1297,10 @@
         <v>34</v>
       </c>
       <c r="BP3">
+        <v>28</v>
+      </c>
+      <c r="BQ3">
         <v>33</v>
-      </c>
-      <c r="BQ3">
-        <v>39</v>
       </c>
       <c r="BR3">
         <v>24</v>
@@ -1273,10 +1309,10 @@
         <v>16</v>
       </c>
       <c r="BT3">
+        <v>12</v>
+      </c>
+      <c r="BU3">
         <v>27</v>
-      </c>
-      <c r="BU3">
-        <v>20</v>
       </c>
       <c r="BV3">
         <v>29</v>
@@ -1285,10 +1321,10 @@
         <v>33</v>
       </c>
       <c r="BX3">
+        <v>27</v>
+      </c>
+      <c r="BY3">
         <v>36</v>
-      </c>
-      <c r="BY3">
-        <v>35</v>
       </c>
       <c r="BZ3">
         <v>24</v>
@@ -1297,15 +1333,15 @@
         <v>35</v>
       </c>
       <c r="CB3">
+        <v>31</v>
+      </c>
+      <c r="CC3">
         <v>30</v>
-      </c>
-      <c r="CC3">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>37</v>
@@ -1313,6 +1349,9 @@
       <c r="C4">
         <v>30</v>
       </c>
+      <c r="D4">
+        <v>22</v>
+      </c>
       <c r="E4">
         <v>39</v>
       </c>
@@ -1322,6 +1361,9 @@
       <c r="G4">
         <v>50</v>
       </c>
+      <c r="H4">
+        <v>42</v>
+      </c>
       <c r="I4">
         <v>45</v>
       </c>
@@ -1331,6 +1373,9 @@
       <c r="K4">
         <v>31</v>
       </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
       <c r="M4">
         <v>40</v>
       </c>
@@ -1340,6 +1385,9 @@
       <c r="O4">
         <v>42</v>
       </c>
+      <c r="P4">
+        <v>36</v>
+      </c>
       <c r="Q4">
         <v>44</v>
       </c>
@@ -1349,6 +1397,9 @@
       <c r="S4">
         <v>29</v>
       </c>
+      <c r="T4">
+        <v>23</v>
+      </c>
       <c r="U4">
         <v>23</v>
       </c>
@@ -1358,6 +1409,9 @@
       <c r="W4">
         <v>30</v>
       </c>
+      <c r="X4">
+        <v>16</v>
+      </c>
       <c r="Y4">
         <v>34</v>
       </c>
@@ -1368,10 +1422,10 @@
         <v>29</v>
       </c>
       <c r="AB4">
+        <v>15</v>
+      </c>
+      <c r="AC4">
         <v>37</v>
-      </c>
-      <c r="AC4">
-        <v>30</v>
       </c>
       <c r="AD4">
         <v>39</v>
@@ -1380,10 +1434,10 @@
         <v>38</v>
       </c>
       <c r="AF4">
+        <v>24</v>
+      </c>
+      <c r="AG4">
         <v>40</v>
-      </c>
-      <c r="AG4">
-        <v>39</v>
       </c>
       <c r="AH4">
         <v>38</v>
@@ -1392,10 +1446,10 @@
         <v>37</v>
       </c>
       <c r="AJ4">
+        <v>25</v>
+      </c>
+      <c r="AK4">
         <v>38</v>
-      </c>
-      <c r="AK4">
-        <v>39</v>
       </c>
       <c r="AL4">
         <v>36</v>
@@ -1404,10 +1458,10 @@
         <v>34</v>
       </c>
       <c r="AN4">
+        <v>20</v>
+      </c>
+      <c r="AO4">
         <v>38</v>
-      </c>
-      <c r="AO4">
-        <v>36</v>
       </c>
       <c r="AP4">
         <v>52</v>
@@ -1416,10 +1470,10 @@
         <v>44</v>
       </c>
       <c r="AR4">
+        <v>38</v>
+      </c>
+      <c r="AS4">
         <v>55</v>
-      </c>
-      <c r="AS4">
-        <v>46</v>
       </c>
       <c r="AT4">
         <v>28</v>
@@ -1428,10 +1482,10 @@
         <v>30</v>
       </c>
       <c r="AV4">
+        <v>22</v>
+      </c>
+      <c r="AW4">
         <v>28</v>
-      </c>
-      <c r="AW4">
-        <v>30</v>
       </c>
       <c r="AX4">
         <v>44</v>
@@ -1440,10 +1494,10 @@
         <v>42</v>
       </c>
       <c r="AZ4">
+        <v>34</v>
+      </c>
+      <c r="BA4">
         <v>44</v>
-      </c>
-      <c r="BA4">
-        <v>43</v>
       </c>
       <c r="BB4">
         <v>39</v>
@@ -1452,10 +1506,10 @@
         <v>45</v>
       </c>
       <c r="BD4">
+        <v>39</v>
+      </c>
+      <c r="BE4">
         <v>41</v>
-      </c>
-      <c r="BE4">
-        <v>47</v>
       </c>
       <c r="BF4">
         <v>44</v>
@@ -1464,10 +1518,10 @@
         <v>42</v>
       </c>
       <c r="BH4">
+        <v>38</v>
+      </c>
+      <c r="BI4">
         <v>45</v>
-      </c>
-      <c r="BI4">
-        <v>44</v>
       </c>
       <c r="BJ4">
         <v>29</v>
@@ -1476,10 +1530,10 @@
         <v>34</v>
       </c>
       <c r="BL4">
+        <v>18</v>
+      </c>
+      <c r="BM4">
         <v>33</v>
-      </c>
-      <c r="BM4">
-        <v>34</v>
       </c>
       <c r="BN4">
         <v>29</v>
@@ -1488,7 +1542,7 @@
         <v>30</v>
       </c>
       <c r="BP4">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="BQ4">
         <v>33</v>
@@ -1500,10 +1554,10 @@
         <v>34</v>
       </c>
       <c r="BT4">
+        <v>22</v>
+      </c>
+      <c r="BU4">
         <v>33</v>
-      </c>
-      <c r="BU4">
-        <v>38</v>
       </c>
       <c r="BV4">
         <v>34</v>
@@ -1512,10 +1566,10 @@
         <v>28</v>
       </c>
       <c r="BX4">
+        <v>12</v>
+      </c>
+      <c r="BY4">
         <v>36</v>
-      </c>
-      <c r="BY4">
-        <v>28</v>
       </c>
       <c r="BZ4">
         <v>27</v>
@@ -1524,15 +1578,15 @@
         <v>31</v>
       </c>
       <c r="CB4">
+        <v>15</v>
+      </c>
+      <c r="CC4">
         <v>30</v>
-      </c>
-      <c r="CC4">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>35</v>
@@ -1540,6 +1594,9 @@
       <c r="C5">
         <v>34</v>
       </c>
+      <c r="D5">
+        <v>34</v>
+      </c>
       <c r="E5">
         <v>37</v>
       </c>
@@ -1549,6 +1606,9 @@
       <c r="G5">
         <v>31</v>
       </c>
+      <c r="H5">
+        <v>29</v>
+      </c>
       <c r="I5">
         <v>42</v>
       </c>
@@ -1558,6 +1618,9 @@
       <c r="K5">
         <v>34</v>
       </c>
+      <c r="L5">
+        <v>30</v>
+      </c>
       <c r="M5">
         <v>36</v>
       </c>
@@ -1567,6 +1630,9 @@
       <c r="O5">
         <v>21</v>
       </c>
+      <c r="P5">
+        <v>19</v>
+      </c>
       <c r="Q5">
         <v>27</v>
       </c>
@@ -1576,6 +1642,9 @@
       <c r="S5">
         <v>20</v>
       </c>
+      <c r="T5">
+        <v>14</v>
+      </c>
       <c r="U5">
         <v>27</v>
       </c>
@@ -1585,6 +1654,9 @@
       <c r="W5">
         <v>41</v>
       </c>
+      <c r="X5">
+        <v>29</v>
+      </c>
       <c r="Y5">
         <v>47</v>
       </c>
@@ -1595,10 +1667,10 @@
         <v>35</v>
       </c>
       <c r="AB5">
+        <v>25</v>
+      </c>
+      <c r="AC5">
         <v>35</v>
-      </c>
-      <c r="AC5">
-        <v>39</v>
       </c>
       <c r="AD5">
         <v>40</v>
@@ -1607,7 +1679,7 @@
         <v>33</v>
       </c>
       <c r="AF5">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="AG5">
         <v>41</v>
@@ -1619,10 +1691,10 @@
         <v>40</v>
       </c>
       <c r="AJ5">
+        <v>36</v>
+      </c>
+      <c r="AK5">
         <v>39</v>
-      </c>
-      <c r="AK5">
-        <v>46</v>
       </c>
       <c r="AL5">
         <v>31</v>
@@ -1631,10 +1703,10 @@
         <v>32</v>
       </c>
       <c r="AN5">
+        <v>24</v>
+      </c>
+      <c r="AO5">
         <v>35</v>
-      </c>
-      <c r="AO5">
-        <v>36</v>
       </c>
       <c r="AP5">
         <v>35</v>
@@ -1643,10 +1715,10 @@
         <v>39</v>
       </c>
       <c r="AR5">
+        <v>33</v>
+      </c>
+      <c r="AS5">
         <v>37</v>
-      </c>
-      <c r="AS5">
-        <v>40</v>
       </c>
       <c r="AT5">
         <v>39</v>
@@ -1655,10 +1727,10 @@
         <v>44</v>
       </c>
       <c r="AV5">
+        <v>40</v>
+      </c>
+      <c r="AW5">
         <v>45</v>
-      </c>
-      <c r="AW5">
-        <v>47</v>
       </c>
       <c r="AX5">
         <v>39</v>
@@ -1667,10 +1739,10 @@
         <v>45</v>
       </c>
       <c r="AZ5">
+        <v>41</v>
+      </c>
+      <c r="BA5">
         <v>42</v>
-      </c>
-      <c r="BA5">
-        <v>47</v>
       </c>
       <c r="BB5">
         <v>29</v>
@@ -1679,10 +1751,10 @@
         <v>26</v>
       </c>
       <c r="BD5">
+        <v>22</v>
+      </c>
+      <c r="BE5">
         <v>32</v>
-      </c>
-      <c r="BE5">
-        <v>28</v>
       </c>
       <c r="BF5">
         <v>36</v>
@@ -1691,10 +1763,10 @@
         <v>49</v>
       </c>
       <c r="BH5">
+        <v>41</v>
+      </c>
+      <c r="BI5">
         <v>37</v>
-      </c>
-      <c r="BI5">
-        <v>49</v>
       </c>
       <c r="BJ5">
         <v>43</v>
@@ -1703,10 +1775,10 @@
         <v>53</v>
       </c>
       <c r="BL5">
+        <v>42</v>
+      </c>
+      <c r="BM5">
         <v>53</v>
-      </c>
-      <c r="BM5">
-        <v>57</v>
       </c>
       <c r="BN5">
         <v>41</v>
@@ -1715,10 +1787,10 @@
         <v>39</v>
       </c>
       <c r="BP5">
+        <v>25</v>
+      </c>
+      <c r="BQ5">
         <v>45</v>
-      </c>
-      <c r="BQ5">
-        <v>43</v>
       </c>
       <c r="BR5">
         <v>31</v>
@@ -1727,10 +1799,10 @@
         <v>25</v>
       </c>
       <c r="BT5">
+        <v>21</v>
+      </c>
+      <c r="BU5">
         <v>36</v>
-      </c>
-      <c r="BU5">
-        <v>31</v>
       </c>
       <c r="BV5">
         <v>28</v>
@@ -1739,10 +1811,10 @@
         <v>33</v>
       </c>
       <c r="BX5">
+        <v>23</v>
+      </c>
+      <c r="BY5">
         <v>35</v>
-      </c>
-      <c r="BY5">
-        <v>36</v>
       </c>
       <c r="BZ5">
         <v>25</v>
@@ -1751,10 +1823,10 @@
         <v>36</v>
       </c>
       <c r="CB5">
+        <v>24</v>
+      </c>
+      <c r="CC5">
         <v>27</v>
-      </c>
-      <c r="CC5">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>